<commit_message>
better formatting for letter grade formula
</commit_message>
<xml_diff>
--- a/Standards based exam generator/Linear Algebra Example Grades.xlsx
+++ b/Standards based exam generator/Linear Algebra Example Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://davidsoncollegenc-my.sharepoint.com/personal/clmerriman_davidson_edu/Documents/Teaching--Course Material and Documents/Linear Algebra/Spring24Reviews To Share/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://davidsoncollegenc-my.sharepoint.com/personal/clmerriman_davidson_edu/Documents/Teaching--Course Material and Documents/Linear Algebra/linear-alg-standards/linear-alg-standards/Standards based exam generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1053" documentId="8_{523429E8-7BA5-FA45-8CBA-2096FCB904FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5CE229-2B1D-9A46-A0BF-43B518E677BD}"/>
+  <xr:revisionPtr revIDLastSave="1067" documentId="8_{523429E8-7BA5-FA45-8CBA-2096FCB904FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB61BA2E-094A-2049-919D-144F76468CBF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homework_1_scores" sheetId="4" r:id="rId1"/>
@@ -590,7 +590,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -692,6 +692,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -751,7 +757,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
@@ -807,6 +813,7 @@
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,7 +827,132 @@
     <cellStyle name="Normal 9" xfId="9" xr:uid="{45416CE9-1585-6947-8196-11EAE957EB51}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1087,10 +1219,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1630,7 +1758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7770B68E-3660-3640-8367-868E941A8C12}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -3684,8 +3812,8 @@
   <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D20" sqref="D20"/>
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4706,55 +4834,55 @@
     <sortCondition ref="B1:B6"/>
   </sortState>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="26" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="12" stopIfTrue="1" operator="equal">
       <formula>COUNTIF($I2:$AD2,"&lt;&gt;")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="13" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="13" stopIfTrue="1" operator="lessThan">
       <formula>0.5*COUNTIF($I2:$AD2,"&lt;&gt;")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D5">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E5">
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="lessThan">
       <formula>2.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" stopIfTrue="1" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F5">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H5">
-    <cfRule type="cellIs" dxfId="18" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>2.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:H5">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:AF5">
-    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="U">
+    <cfRule type="containsText" dxfId="30" priority="3" operator="containsText" text="U">
       <formula>NOT(ISERROR(SEARCH("U",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="29" priority="4" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="DN">
+    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="DN">
       <formula>NOT(ISERROR(SEARCH("DN",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4766,9 +4894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CY9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BN2" sqref="BN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5084,7 +5212,7 @@
       <c r="CX1" s="9"/>
       <c r="CY1" s="9"/>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>170</v>
       </c>
@@ -5289,7 +5417,7 @@
         <v>0</v>
       </c>
       <c r="CL2" s="17">
-        <f>(SUM($F2:$AB2)-SMALL($F2:$AB2,2)-SMALL($F2:$AB2,1))/(3*(COUNTA($F2:$AB2)-2))</f>
+        <f>(SUM($F2:$AB2) - SMALL($F2:$AB2,1) - SMALL($F2:$AB2,2)) / (3 * (COUNTA($F2:$AB2) - 2))</f>
         <v>1</v>
       </c>
       <c r="CM2" s="17">
@@ -5305,7 +5433,7 @@
         <v>0.9642857142857143</v>
       </c>
       <c r="CP2" s="15">
-        <f>SUM($BN2:$CK2)/(24-COUNTBLANK(BN2:CK2))</f>
+        <f>AVERAGEIF($BN2:$CK2, "&lt;&gt;")</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="CQ2" s="19">
@@ -5313,22 +5441,22 @@
         <v>0.88394088669950743</v>
       </c>
       <c r="CR2" t="str">
-        <f t="shared" ref="CR2:CR5" si="2">IF($CQ2&gt;=0.93,"A",IF($CQ2&gt;=0.9,"A-",IF($CQ2&gt;=0.87,"B+",IF($CQ2&gt;=0.83,"B",IF($CQ2&gt;=0.8,"B-",IF($CQ2&gt;=0.77,"C+",IF($CQ2&gt;=0.73,"C",IF($CQ2&gt;=0.7,"C-",IF($CQ2&gt;=0.67,"D+",IF($CQ2&gt;=0.6,"D","F"))))))))))</f>
+        <f>LOOKUP($CQ2, {0,0.6,0.67,0.7,0.73,0.77,0.8,0.83,0.87,0.9,0.93}, {"F","D","D+","C-","C","C+","B-","B","B+","A-","A"})</f>
         <v>B+</v>
       </c>
       <c r="CS2" s="23">
         <f>$CL2*0.04+$CM2*0.05+$CN2*0.15+$CO2*0.16+(SUM($BN2:$CA2))/14*0.6</f>
         <v>0.89822660098522167</v>
       </c>
-      <c r="CT2" t="str">
-        <f t="shared" ref="CT2:CT5" si="3">IF($CS2&gt;=0.93,"A",IF($CS2&gt;=0.9,"A-",IF($CS2&gt;=0.87,"B+",IF($CS2&gt;=0.83,"B",IF($CS2&gt;=0.8,"B-",IF($CS2&gt;=0.77,"C+",IF($CS2&gt;=0.73,"C",IF($CS2&gt;=0.7,"C-",IF($CS2&gt;=0.67,"D+",IF($CS2&gt;=0.6,"D","F"))))))))))</f>
+      <c r="CT2" s="49" t="str">
+        <f>LOOKUP($CS2, {0,0.6,0.67,0.7,0.73,0.77,0.8,0.83,0.87,0.9,0.93}, {"F","D","D+","C-","C","C+","B-","B","B+","A-","A"})</f>
         <v>B+</v>
       </c>
       <c r="CU2" s="23"/>
       <c r="CX2" s="11"/>
       <c r="CY2" s="38"/>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>171</v>
       </c>
@@ -5533,7 +5661,7 @@
         <v>0</v>
       </c>
       <c r="CL3" s="17">
-        <f t="shared" ref="CL3:CL5" si="4">(SUM($F3:$AB3)-SMALL($F3:$AB3,2)-SMALL($F3:$AB3,1))/(3*(COUNTA($F3:$AB3)-2))</f>
+        <f t="shared" ref="CL3:CL5" si="2">(SUM($F3:$AB3) - SMALL($F3:$AB3,1) - SMALL($F3:$AB3,2)) / (3 * (COUNTA($F3:$AB3) - 2))</f>
         <v>1</v>
       </c>
       <c r="CM3" s="17">
@@ -5541,38 +5669,38 @@
         <v>1</v>
       </c>
       <c r="CN3" s="36">
-        <f t="shared" ref="CN3:CN5" si="5">AVERAGE($AU3:$BD3)</f>
+        <f t="shared" ref="CN3:CN5" si="3">AVERAGE($AU3:$BD3)</f>
         <v>0.86206896551724133</v>
       </c>
       <c r="CO3" s="36">
-        <f t="shared" ref="CO3:CO5" si="6">AVERAGE(BE3:BM3)</f>
+        <f t="shared" ref="CO3:CO5" si="4">AVERAGE(BE3:BM3)</f>
         <v>0.8571428571428571</v>
       </c>
       <c r="CP3" s="15">
-        <f t="shared" ref="CP3:CP5" si="7">SUM($BN3:$CK3)/(24-COUNTBLANK(BN3:CK3))</f>
+        <f t="shared" ref="CP3:CP5" si="5">AVERAGEIF($BN3:$CK3, "&lt;&gt;")</f>
         <v>0.79166666666666663</v>
       </c>
       <c r="CQ3" s="19">
-        <f t="shared" ref="CQ3:CQ5" si="8">$CL3*0.04+$CM3*0.05+$CN3*0.15+$CO3*0.16+$CP3*0.6</f>
+        <f t="shared" ref="CQ3:CQ5" si="6">$CL3*0.04+$CM3*0.05+$CN3*0.15+$CO3*0.16+$CP3*0.6</f>
         <v>0.83145320197044326</v>
       </c>
       <c r="CR3" t="str">
-        <f t="shared" si="2"/>
+        <f>LOOKUP($CQ3, {0,0.6,0.67,0.7,0.73,0.77,0.8,0.83,0.87,0.9,0.93}, {"F","D","D+","C-","C","C+","B-","B","B+","A-","A"})</f>
         <v>B</v>
       </c>
       <c r="CS3" s="23">
-        <f t="shared" ref="CS3:CS5" si="9">$CL3*0.04+$CM3*0.05+$CN3*0.15+$CO3*0.16+(SUM($BN3:$CA3))/14*0.6</f>
+        <f t="shared" ref="CS3:CS5" si="7">$CL3*0.04+$CM3*0.05+$CN3*0.15+$CO3*0.16+(SUM($BN3:$CA3))/14*0.6</f>
         <v>0.8278817733990147</v>
       </c>
-      <c r="CT3" t="str">
-        <f t="shared" si="3"/>
+      <c r="CT3" s="49" t="str">
+        <f>LOOKUP($CS3, {0,0.6,0.67,0.7,0.73,0.77,0.8,0.83,0.87,0.9,0.93}, {"F","D","D+","C-","C","C+","B-","B","B+","A-","A"})</f>
         <v>B-</v>
       </c>
       <c r="CU3" s="23"/>
       <c r="CX3" s="11"/>
       <c r="CY3" s="38"/>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>172</v>
       </c>
@@ -5777,7 +5905,7 @@
         <v>0</v>
       </c>
       <c r="CL4" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="CM4" s="17">
@@ -5785,38 +5913,38 @@
         <v>1</v>
       </c>
       <c r="CN4" s="36">
+        <f t="shared" si="3"/>
+        <v>0.89655172413793105</v>
+      </c>
+      <c r="CO4" s="36">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="CP4" s="15">
         <f t="shared" si="5"/>
-        <v>0.89655172413793105</v>
-      </c>
-      <c r="CO4" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="CQ4" s="19">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="CP4" s="15">
+        <v>0.83448275862068955</v>
+      </c>
+      <c r="CR4" t="str">
+        <f>LOOKUP($CQ4, {0,0.6,0.67,0.7,0.73,0.77,0.8,0.83,0.87,0.9,0.93}, {"F","D","D+","C-","C","C+","B-","B","B+","A-","A"})</f>
+        <v>B</v>
+      </c>
+      <c r="CS4" s="23">
         <f t="shared" si="7"/>
-        <v>0.75</v>
-      </c>
-      <c r="CQ4" s="19">
-        <f t="shared" si="8"/>
-        <v>0.83448275862068955</v>
-      </c>
-      <c r="CR4" t="str">
-        <f t="shared" si="2"/>
-        <v>B</v>
-      </c>
-      <c r="CS4" s="23">
-        <f t="shared" si="9"/>
         <v>0.94162561576354675</v>
       </c>
-      <c r="CT4" t="str">
-        <f t="shared" si="3"/>
+      <c r="CT4" s="49" t="str">
+        <f>LOOKUP($CS4, {0,0.6,0.67,0.7,0.73,0.77,0.8,0.83,0.87,0.9,0.93}, {"F","D","D+","C-","C","C+","B-","B","B+","A-","A"})</f>
         <v>A</v>
       </c>
       <c r="CU4" s="23"/>
       <c r="CX4" s="11"/>
       <c r="CY4" s="38"/>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>173</v>
       </c>
@@ -6021,7 +6149,7 @@
         <v>1</v>
       </c>
       <c r="CL5" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="CM5" s="17">
@@ -6029,31 +6157,31 @@
         <v>1</v>
       </c>
       <c r="CN5" s="36">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CO5" s="36">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="CP5" s="15">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="CO5" s="36">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="CQ5" s="19">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="CP5" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="CR5" t="str">
+        <f>LOOKUP($CQ5, {0,0.6,0.67,0.7,0.73,0.77,0.8,0.83,0.87,0.9,0.93}, {"F","D","D+","C-","C","C+","B-","B","B+","A-","A"})</f>
+        <v>B-</v>
+      </c>
+      <c r="CS5" s="23">
         <f t="shared" si="7"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="CQ5" s="19">
-        <f t="shared" si="8"/>
-        <v>0.8</v>
-      </c>
-      <c r="CR5" t="str">
-        <f t="shared" si="2"/>
-        <v>B-</v>
-      </c>
-      <c r="CS5" s="23">
-        <f t="shared" si="9"/>
         <v>0.82857142857142851</v>
       </c>
-      <c r="CT5" t="str">
-        <f t="shared" si="3"/>
+      <c r="CT5" s="49" t="str">
+        <f>LOOKUP($CS5, {0,0.6,0.67,0.7,0.73,0.77,0.8,0.83,0.87,0.9,0.93}, {"F","D","D+","C-","C","C+","B-","B","B+","A-","A"})</f>
         <v>B-</v>
       </c>
       <c r="CU5" s="23"/>
@@ -6108,44 +6236,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CN2:CO5">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="lessThan">
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="lessThan">
       <formula>0.6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP2:CP5">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR2:CR5 CT2:CT5 CV2:CV5">
-    <cfRule type="cellIs" dxfId="8" priority="34" operator="equal">
+  <conditionalFormatting sqref="CV2:CV5 CR2:CR5">
+    <cfRule type="cellIs" dxfId="22" priority="42" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="35" operator="containsText" text="D+">
+    <cfRule type="containsText" dxfId="21" priority="40" operator="containsText" text="D+">
       <formula>NOT(ISERROR(SEARCH("D+",CR2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="41" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="37" operator="containsText" text="C">
+    <cfRule type="containsText" dxfId="19" priority="39" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",CR2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="38" operator="containsText" text="B-">
+    <cfRule type="containsText" dxfId="18" priority="38" operator="containsText" text="B-">
       <formula>NOT(ISERROR(SEARCH("B-",CR2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="39" operator="containsText" text="B+">
+    <cfRule type="containsText" dxfId="17" priority="36" operator="containsText" text="B+">
       <formula>NOT(ISERROR(SEARCH("B+",CR2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="37" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="41" operator="containsText" text="A-">
+    <cfRule type="containsText" dxfId="15" priority="35" stopIfTrue="1" operator="containsText" text="A-">
       <formula>NOT(ISERROR(SEARCH("A-",CR2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="42" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="14" priority="34" stopIfTrue="1" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",CR2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>